<commit_message>
first done portfolio data power bi
</commit_message>
<xml_diff>
--- a/.xlsx/full_stock_classification.xlsx
+++ b/.xlsx/full_stock_classification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\twan-projects\py-app\.xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8696A608-6C33-4EE8-8C33-CB14CFBA827F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECAB6F6E-19D7-4386-B3EB-611C051CB142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22046" yWindow="-103" windowWidth="22149" windowHeight="13200" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="quarter_stock_list" sheetId="5" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17966" uniqueCount="1759">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17978" uniqueCount="1768">
   <si>
     <t>PGC</t>
   </si>
@@ -5326,13 +5326,40 @@
   </si>
   <si>
     <t>o</t>
+  </si>
+  <si>
+    <t>small_6stocks</t>
+  </si>
+  <si>
+    <t>portfolio</t>
+  </si>
+  <si>
+    <t>small_10stocks</t>
+  </si>
+  <si>
+    <t>large_6stocks</t>
+  </si>
+  <si>
+    <t>medium_6stocks</t>
+  </si>
+  <si>
+    <t>SMALL10</t>
+  </si>
+  <si>
+    <t>SMALL6</t>
+  </si>
+  <si>
+    <t>MEDIUM6</t>
+  </si>
+  <si>
+    <t>LARGE6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5352,6 +5379,12 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -81244,16 +81277,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEC4401C-D304-4750-8CED-A9CF758C9679}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -81706,7 +81739,64 @@
         <v>1</v>
       </c>
     </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>1761</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1760</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1764</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>1759</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1760</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1765</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>1763</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1760</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1766</v>
+      </c>
+      <c r="D35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>1762</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1760</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1767</v>
+      </c>
+      <c r="D36">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -81715,7 +81805,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD58B990-4E93-4226-B2C3-FA35F0465DC7}">
   <dimension ref="A1:B495"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A482" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A482" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I489" sqref="I489"/>
     </sheetView>
   </sheetViews>

</xml_diff>